<commit_message>
TestRail API : Update Test Cases with Title
</commit_message>
<xml_diff>
--- a/src/test/resources/legionTestCases.xlsx
+++ b/src/test/resources/legionTestCases.xlsx
@@ -18,7 +18,9 @@
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Defects to Verified'!$A$1:$B$91</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Scope of Build Qual'!$A$1:$Z$53</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Scope of Build Qual'!$A$1:$Z$53</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Scope of Build Qual'!$A$1:$Z$53</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Defects to Verified'!$A$1:$B$91</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Defects to Verified'!$A$1:$B$91</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -3736,14 +3738,14 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I157:J158 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="77.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="76.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4102,24 +4104,24 @@
   </sheetPr>
   <dimension ref="A1:AB65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="I157" activeCellId="0" sqref="I157:J158"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="28" min="10" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="70.3316326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="28" min="10" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4180,7 +4182,7 @@
       <c r="AA1" s="7"/>
       <c r="AB1" s="7"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -7600,7 +7602,7 @@
       <c r="AA74" s="7"/>
       <c r="AB74" s="7"/>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
         <v>7</v>
       </c>
@@ -10240,19 +10242,19 @@
   <dimension ref="A1:Z101"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I157:J158 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="72.2193877551021"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="71.4081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13988,14 +13990,14 @@
   <dimension ref="A1:X91"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I157:J158 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14818,14 +14820,14 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I157:J158 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="101.785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="100.566326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
TestRail API : add/update/remove Test Cases with Title
</commit_message>
<xml_diff>
--- a/src/test/resources/legionTestCases.xlsx
+++ b/src/test/resources/legionTestCases.xlsx
@@ -253,7 +253,8 @@
     <t xml:space="preserve">User Must have The Credentials for Login into the Application.
 Environment URL:
 Username:
-Password:</t>
+Password:
+Added A Line</t>
   </si>
   <si>
     <t xml:space="preserve">User must have browser (Chrome) installed to launch the application
@@ -4107,7 +4108,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4182,7 +4183,7 @@
       <c r="AA1" s="7"/>
       <c r="AB1" s="7"/>
     </row>
-    <row r="2" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>